<commit_message>
Add Test data and test codes.
</commit_message>
<xml_diff>
--- a/TableReader/src/test/TestData/GetTable_Test.xlsx
+++ b/TableReader/src/test/TestData/GetTable_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21090" windowHeight="8280" tabRatio="863" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21090" windowHeight="8280" tabRatio="863" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="GetTable_test_001" sheetId="13" r:id="rId1"/>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -877,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Update TableReader.dll. Add method to read values from the row specified by the argument. Update test data and add test about the GetTable() method. Change the version of the dll to ver.0.5.0.
</commit_message>
<xml_diff>
--- a/TableReader/src/test/TestData/GetTable_Test.xlsx
+++ b/TableReader/src/test/TestData/GetTable_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21090" windowHeight="8280" tabRatio="863" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21090" windowHeight="8280" tabRatio="863" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="GetTable_test_001" sheetId="13" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="GetTable_test_004" sheetId="16" r:id="rId4"/>
     <sheet name="GetTable_test_005" sheetId="17" r:id="rId5"/>
     <sheet name="GetTable_test_006" sheetId="19" r:id="rId6"/>
+    <sheet name="GetTable_test_007" sheetId="20" r:id="rId7"/>
+    <sheet name="GetTable_test_008" sheetId="21" r:id="rId8"/>
+    <sheet name="GetTable_test_009" sheetId="22" r:id="rId9"/>
+    <sheet name="GetTable_test_010" sheetId="23" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="22">
   <si>
     <t>Item_r_001_c_002</t>
   </si>
@@ -96,6 +100,10 @@
   </si>
   <si>
     <t>Item_r_001_c_001</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Item_r_002_c_002</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -427,7 +435,7 @@
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F7"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -515,12 +523,102 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -961,4 +1059,274 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>